<commit_message>
17.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/March/All Details/16.03.2020/MC Balance Transfer March 2020.xlsx
+++ b/2020/March/All Details/16.03.2020/MC Balance Transfer March 2020.xlsx
@@ -1103,7 +1103,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1115,7 +1115,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1138,14 +1138,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1453,9 +1453,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4610,7 +4610,7 @@
       <c r="A44" s="120"/>
       <c r="B44" s="121"/>
       <c r="C44" s="122">
-        <v>8903</v>
+        <v>4678</v>
       </c>
       <c r="D44" s="123"/>
       <c r="E44" s="3"/>
@@ -5072,7 +5072,7 @@
       </c>
       <c r="B51" s="32"/>
       <c r="C51" s="73">
-        <v>481030</v>
+        <v>485255</v>
       </c>
       <c r="D51" s="74" t="s">
         <v>94</v>

</xml_diff>